<commit_message>
modify and send to git
</commit_message>
<xml_diff>
--- a/MadisonSeleniumPOM/src/test/resources/madsion.xlsx
+++ b/MadisonSeleniumPOM/src/test/resources/madsion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -70,10 +70,10 @@
     <t>mrrobot</t>
   </si>
   <si>
-    <t>anonymousghost789458@gmail.com</t>
-  </si>
-  <si>
     <t>edwardsnowdan999@gmail.com</t>
+  </si>
+  <si>
+    <t>anonymousghost712@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -438,7 +438,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -456,7 +456,6 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -471,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -516,7 +515,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -536,7 +535,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
add reports, screenshots of registration test to github
</commit_message>
<xml_diff>
--- a/MadisonSeleniumPOM/src/test/resources/madsion.xlsx
+++ b/MadisonSeleniumPOM/src/test/resources/madsion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>emailid</t>
   </si>
@@ -70,13 +70,10 @@
     <t>mrrobot</t>
   </si>
   <si>
-    <t>anonymousghost7323@gmail.com</t>
-  </si>
-  <si>
-    <t>edwardsnowdan939@gmail.com</t>
-  </si>
-  <si>
-    <t>anonymousghost7453@gmail.com</t>
+    <t>edwardsnowdan@gmail.com</t>
+  </si>
+  <si>
+    <t>anonymousghost77@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -421,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -441,9 +438,9 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -474,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -519,7 +516,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -539,7 +536,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -550,10 +547,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
update registration test screenshot and extent report.
</commit_message>
<xml_diff>
--- a/MadisonSeleniumPOM/src/test/resources/madsion.xlsx
+++ b/MadisonSeleniumPOM/src/test/resources/madsion.xlsx
@@ -73,7 +73,7 @@
     <t>edwardsnowdan@gmail.com</t>
   </si>
   <si>
-    <t>anonymousghost80@gmail.com</t>
+    <t>anonymousghostpvg@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>

</xml_diff>